<commit_message>
Modified files to add new competitions
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -4,19 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sussex011017" sheetId="1" r:id="rId1"/>
     <sheet name="Birm150417" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="NWOpen211017" sheetId="3" r:id="rId3"/>
+    <sheet name="ScotOp151017" sheetId="4" r:id="rId4"/>
+    <sheet name="Newham071017" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="631">
   <si>
     <t> 1 </t>
   </si>
@@ -1129,13 +1131,793 @@
   </si>
   <si>
     <t>Country</t>
+  </si>
+  <si>
+    <t>Houldsworth, Alastair</t>
+  </si>
+  <si>
+    <t>58848 </t>
+  </si>
+  <si>
+    <t>Belfast </t>
+  </si>
+  <si>
+    <t>GBR </t>
+  </si>
+  <si>
+    <t>Wallace, Luke</t>
+  </si>
+  <si>
+    <t>124710 </t>
+  </si>
+  <si>
+    <t>Grosvenor </t>
+  </si>
+  <si>
+    <t>McMullan, Finn</t>
+  </si>
+  <si>
+    <t>117710 </t>
+  </si>
+  <si>
+    <t>Grosvenor / Fence Like An Olympian </t>
+  </si>
+  <si>
+    <t>Sigurdsson, Daniel</t>
+  </si>
+  <si>
+    <t>125198 </t>
+  </si>
+  <si>
+    <t>Cockburn, Robbie</t>
+  </si>
+  <si>
+    <t>115825 </t>
+  </si>
+  <si>
+    <t>Connery, Jonathan</t>
+  </si>
+  <si>
+    <t>121587 </t>
+  </si>
+  <si>
+    <t>IRL </t>
+  </si>
+  <si>
+    <t>Thompson, Michael</t>
+  </si>
+  <si>
+    <t>121243 </t>
+  </si>
+  <si>
+    <t>Lisburn Gladiators </t>
+  </si>
+  <si>
+    <t>Luney, Rowan</t>
+  </si>
+  <si>
+    <t>125163 </t>
+  </si>
+  <si>
+    <t>RBAI / Fence Like An Olympian </t>
+  </si>
+  <si>
+    <t>McKay, Matthew</t>
+  </si>
+  <si>
+    <t>119635 </t>
+  </si>
+  <si>
+    <t>Salter, Duncan</t>
+  </si>
+  <si>
+    <t>114157 </t>
+  </si>
+  <si>
+    <t>Brian Boru / Pembroke </t>
+  </si>
+  <si>
+    <t>McEvoy, Mark</t>
+  </si>
+  <si>
+    <t>94691 </t>
+  </si>
+  <si>
+    <t>Leung, Chung Hang</t>
+  </si>
+  <si>
+    <t>134866 </t>
+  </si>
+  <si>
+    <t>Ulster University </t>
+  </si>
+  <si>
+    <t>White, David</t>
+  </si>
+  <si>
+    <t>90016 </t>
+  </si>
+  <si>
+    <t>Boyd, Daniel</t>
+  </si>
+  <si>
+    <t>125034 </t>
+  </si>
+  <si>
+    <t>Graham, Stuart</t>
+  </si>
+  <si>
+    <t>128055 </t>
+  </si>
+  <si>
+    <t>BFA_ID</t>
+  </si>
+  <si>
+    <t>COOK, Keith</t>
+  </si>
+  <si>
+    <t>93338 </t>
+  </si>
+  <si>
+    <t>Salle Holyrood </t>
+  </si>
+  <si>
+    <t>DOUGLAS, Jack</t>
+  </si>
+  <si>
+    <t>112508 </t>
+  </si>
+  <si>
+    <t>JONES, Alexander</t>
+  </si>
+  <si>
+    <t>101015 </t>
+  </si>
+  <si>
+    <t>Salle Kiss Fencing Club </t>
+  </si>
+  <si>
+    <t>WOOLLARD, Jonathan</t>
+  </si>
+  <si>
+    <t>113590 </t>
+  </si>
+  <si>
+    <t>RUSSELL, Iain</t>
+  </si>
+  <si>
+    <t>94901 </t>
+  </si>
+  <si>
+    <t>MOLLARD, Christopher</t>
+  </si>
+  <si>
+    <t>102598 </t>
+  </si>
+  <si>
+    <t>Saxon Fencing Club </t>
+  </si>
+  <si>
+    <t>ARBELET, Alexandre</t>
+  </si>
+  <si>
+    <t>124482 </t>
+  </si>
+  <si>
+    <t>SUI </t>
+  </si>
+  <si>
+    <t>ALDERMAN, Shaun</t>
+  </si>
+  <si>
+    <t>110520 </t>
+  </si>
+  <si>
+    <t>SHARMAN, Conor</t>
+  </si>
+  <si>
+    <t>53920 </t>
+  </si>
+  <si>
+    <t>Loughborough Students Union </t>
+  </si>
+  <si>
+    <t>SCHLINDWEIN, Alex</t>
+  </si>
+  <si>
+    <t>99229 </t>
+  </si>
+  <si>
+    <t>Cambridge University Fencing Club </t>
+  </si>
+  <si>
+    <t>MCANDREW, Finlay</t>
+  </si>
+  <si>
+    <t>117377 </t>
+  </si>
+  <si>
+    <t>MORRISON, Duncan</t>
+  </si>
+  <si>
+    <t>105639 </t>
+  </si>
+  <si>
+    <t>DOOTSON, nick</t>
+  </si>
+  <si>
+    <t>37089 </t>
+  </si>
+  <si>
+    <t>AMBELEZ, Mauro</t>
+  </si>
+  <si>
+    <t>112075 </t>
+  </si>
+  <si>
+    <t>Laszlo </t>
+  </si>
+  <si>
+    <t>BROUGHTON, Charlie</t>
+  </si>
+  <si>
+    <t>112105 </t>
+  </si>
+  <si>
+    <t>STANBRIDGE, paul</t>
+  </si>
+  <si>
+    <t>57596 </t>
+  </si>
+  <si>
+    <t>HILL, Michael</t>
+  </si>
+  <si>
+    <t>97356 </t>
+  </si>
+  <si>
+    <t>Dundee University Fencing Club </t>
+  </si>
+  <si>
+    <t>CUDWORTH, Mark</t>
+  </si>
+  <si>
+    <t>53517 </t>
+  </si>
+  <si>
+    <t>BANKS, Joe</t>
+  </si>
+  <si>
+    <t>46075 </t>
+  </si>
+  <si>
+    <t>FIELDING, Iain</t>
+  </si>
+  <si>
+    <t>106672 </t>
+  </si>
+  <si>
+    <t>West Fife Fencing Club </t>
+  </si>
+  <si>
+    <t>LAUCHLAN, Mark</t>
+  </si>
+  <si>
+    <t>100245 </t>
+  </si>
+  <si>
+    <t>Wallace Fencing Academy </t>
+  </si>
+  <si>
+    <t>STEELE, Gabriel</t>
+  </si>
+  <si>
+    <t>111406 </t>
+  </si>
+  <si>
+    <t>Salle Holyrood / Salle Holyrood Fencing Club </t>
+  </si>
+  <si>
+    <t>EUSTON, Matthew</t>
+  </si>
+  <si>
+    <t>93842 </t>
+  </si>
+  <si>
+    <t>BOWER, Edward</t>
+  </si>
+  <si>
+    <t>43857 </t>
+  </si>
+  <si>
+    <t>DOLAN, George</t>
+  </si>
+  <si>
+    <t>95138 </t>
+  </si>
+  <si>
+    <t>Glasgow West End Fencing Club </t>
+  </si>
+  <si>
+    <t>HALL, Mark</t>
+  </si>
+  <si>
+    <t>128202 </t>
+  </si>
+  <si>
+    <t>Birmingham Fencing Club </t>
+  </si>
+  <si>
+    <t>MCARTHUR, Sam</t>
+  </si>
+  <si>
+    <t>113026 </t>
+  </si>
+  <si>
+    <t>Heriot Watt University Fencing Club </t>
+  </si>
+  <si>
+    <t>BRYSON, Louis</t>
+  </si>
+  <si>
+    <t>119695 </t>
+  </si>
+  <si>
+    <t>MILNE, Kev</t>
+  </si>
+  <si>
+    <t>93452 </t>
+  </si>
+  <si>
+    <t>CRAWFORD, Angus</t>
+  </si>
+  <si>
+    <t>117375 </t>
+  </si>
+  <si>
+    <t>HAMILTON, Gareth</t>
+  </si>
+  <si>
+    <t>100242 </t>
+  </si>
+  <si>
+    <t>GARCIA, Jesus</t>
+  </si>
+  <si>
+    <t>127665 </t>
+  </si>
+  <si>
+    <t>Imperial College Union F.c </t>
+  </si>
+  <si>
+    <t>ESP </t>
+  </si>
+  <si>
+    <t>AHMAD, Mortaz</t>
+  </si>
+  <si>
+    <t>134938 </t>
+  </si>
+  <si>
+    <t>GER </t>
+  </si>
+  <si>
+    <t>SCHUESSLER, Benedikt</t>
+  </si>
+  <si>
+    <t>137414 </t>
+  </si>
+  <si>
+    <t>DOCHERTY, John</t>
+  </si>
+  <si>
+    <t>116958 </t>
+  </si>
+  <si>
+    <t>ROBERTS, Dylan</t>
+  </si>
+  <si>
+    <t>112058 </t>
+  </si>
+  <si>
+    <t>MCEWAN, Mike</t>
+  </si>
+  <si>
+    <t>95171 </t>
+  </si>
+  <si>
+    <t>GUNN, Chris</t>
+  </si>
+  <si>
+    <t>136132 </t>
+  </si>
+  <si>
+    <t>St Andrews University Fencing Club </t>
+  </si>
+  <si>
+    <t>REID, Callum</t>
+  </si>
+  <si>
+    <t>136129 </t>
+  </si>
+  <si>
+    <t>MUNCASTER, Douglas</t>
+  </si>
+  <si>
+    <t>131157 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BARWELL </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Peter </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ZFW FENCING CLUB </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BILLING </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Matthew </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TRURO FENCING CLUB </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MINOTT </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kamal </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NEWHAM SWORDS </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ROBINSON </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Daniel </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> HEREFORDSHIRE FENCING CLUB </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RAI </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rajan </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ROSSI </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lorenzo </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SALLE BOSTON </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PAGE </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> James </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FENCERS CLUB LONDON </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LENNON </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Christopher </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LEWIS </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Celyn </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> GWENT SWORD CLUB </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SHARMAN </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Conor </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LOUGHBOROUGH UNIVERSITY </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CORLETT </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thomas </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> YOUNGBLOOD </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Henry </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PALLIER </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sebastian </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ALDERMAN </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Shaun </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SALLE HOLYROOD </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PRICE </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> William </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SAXON FENCING CLUB </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MOLLARD </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> JOLLEY </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Isaac </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CHICHESTER FENCING CLUB </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> OSTACCHINI </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Glen </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BIRD </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Harry </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> STANDEN </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> David </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ABIDOGUN </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kola </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> GROSVENOR </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Owen </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PAUL DAVIS FENCING ACADEMY </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> HOWLETT </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Edmund </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SHEFFIELD BUCCANEERS FENCING CLUB </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BROWN </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bomba </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CYRANO FENCING CLUB </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MACCHIAROLA </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Alessandro </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ANDREWS </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ben </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MORT </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Nicholas </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> JOY </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> GUENNOU </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Louis </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ESCRIME ACADEMY </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> WILSON </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Samuel </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MARROQUIN </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Diego </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SALLE PAUL FENCING CLUB </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> UDRZAL </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Benjamin </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> AUSTIN </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kiron </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RIDSDALE </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ethan </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RUSSELL SWORDS </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CHENG </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Vinton </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> OXFORD UNIVERSTIY FENCING CLUB </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DEVITT </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ronnie </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> GILLMAN </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> John </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LOWEN </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Paul </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> THAKKAR </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pranav </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CROMIE </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Eoghan </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SERGEN </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hilmi </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> VAN AARSEN </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Geert </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> THANTHULAGE </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Janith </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> COWLEY </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FITZGERALD </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> GURNSEY </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> HARRINGTON-JOHNSON </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dale </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FIGHTING FIT FENCING CLUB </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> KOVAR </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TAN </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gerald </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> YUN </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lok </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LONDON FENCING CLUB </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BRASTED </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FIHOSY </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LI </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Weiqi </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> HARDEN </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PARKER </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kevin </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ARMY FENCING UNION </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1148,8 +1930,20 @@
       <color rgb="FF000000"/>
       <name val="Times"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1180,8 +1974,38 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFD700"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF888888"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA67D3D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFAFAD2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEEE8AA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -1189,11 +2013,91 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFD2B48C"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFD2B48C"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FFD2B48C"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFD2B48C"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFD2B48C"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFD2B48C"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFD2B48C"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFD2B48C"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFD2B48C"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFD2B48C"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFD2B48C"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFD2B48C"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -1220,6 +2124,70 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2006,8 +2974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4030,12 +4998,1965 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="5.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" style="9" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" t="s">
+        <v>410</v>
+      </c>
+      <c r="D1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>371</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>372</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>373</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="13">
+        <v>2</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>375</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>376</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>377</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="16">
+        <v>3</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>378</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>379</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>380</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="16">
+        <v>3</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>381</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>382</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>377</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="19">
+        <v>5</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>383</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>384</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>380</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="22">
+        <v>6</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>385</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>386</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>377</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="19">
+        <v>7</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>388</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>389</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>390</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="22">
+        <v>8</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>391</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>392</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>393</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="19">
+        <v>9</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>394</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>395</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>393</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="22">
+        <v>10</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>396</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>397</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>398</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="19">
+        <v>11</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>399</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>400</v>
+      </c>
+      <c r="D12" s="20"/>
+      <c r="E12" s="21"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="22">
+        <v>12</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>401</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>402</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>403</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="19">
+        <v>13</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>404</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>405</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>373</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="22">
+        <v>14</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>406</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>407</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>403</v>
+      </c>
+      <c r="E15" s="24" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="25">
+        <v>15</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>408</v>
+      </c>
+      <c r="C16" s="26" t="s">
+        <v>409</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>403</v>
+      </c>
+      <c r="E16" s="27" t="s">
+        <v>374</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="9"/>
+    <col min="4" max="4" width="40.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" t="s">
+        <v>410</v>
+      </c>
+      <c r="D1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>411</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>412</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>413</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="13">
+        <v>2</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>414</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>415</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>413</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="16">
+        <v>3</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>416</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>417</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>418</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="16">
+        <v>3</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>419</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>420</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>413</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="19">
+        <v>5</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>421</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>422</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>413</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="22">
+        <v>6</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>423</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>424</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>425</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="19">
+        <v>7</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>426</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>427</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>413</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="22">
+        <v>8</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>429</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>430</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>413</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="19">
+        <v>9</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>431</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>432</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>433</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="22">
+        <v>10</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>434</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>435</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>436</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="19">
+        <v>11</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>437</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>438</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>413</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="22">
+        <v>12</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>439</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>440</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>413</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="19">
+        <v>13</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>441</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>442</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>413</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="22">
+        <v>14</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>443</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>444</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>445</v>
+      </c>
+      <c r="E15" s="24" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="19">
+        <v>15</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>446</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>447</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>413</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="22">
+        <v>16</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>448</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>449</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>413</v>
+      </c>
+      <c r="E17" s="24" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="19">
+        <v>17</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>450</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>451</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>452</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="22">
+        <v>18</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>453</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>454</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>418</v>
+      </c>
+      <c r="E19" s="24" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="19">
+        <v>19</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>455</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>456</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>425</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="22">
+        <v>20</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>457</v>
+      </c>
+      <c r="C21" s="23" t="s">
+        <v>458</v>
+      </c>
+      <c r="D21" s="23" t="s">
+        <v>459</v>
+      </c>
+      <c r="E21" s="24" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="19">
+        <v>21</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>460</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>461</v>
+      </c>
+      <c r="D22" s="20" t="s">
+        <v>462</v>
+      </c>
+      <c r="E22" s="21" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="22">
+        <v>22</v>
+      </c>
+      <c r="B23" s="23" t="s">
+        <v>463</v>
+      </c>
+      <c r="C23" s="23" t="s">
+        <v>464</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>465</v>
+      </c>
+      <c r="E23" s="24" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="19">
+        <v>23</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>466</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>467</v>
+      </c>
+      <c r="D24" s="20" t="s">
+        <v>462</v>
+      </c>
+      <c r="E24" s="21" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="22">
+        <v>24</v>
+      </c>
+      <c r="B25" s="23" t="s">
+        <v>468</v>
+      </c>
+      <c r="C25" s="23" t="s">
+        <v>469</v>
+      </c>
+      <c r="D25" s="23" t="s">
+        <v>413</v>
+      </c>
+      <c r="E25" s="24" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="19">
+        <v>25</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>470</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>471</v>
+      </c>
+      <c r="D26" s="20" t="s">
+        <v>472</v>
+      </c>
+      <c r="E26" s="21" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="22">
+        <v>26</v>
+      </c>
+      <c r="B27" s="23" t="s">
+        <v>473</v>
+      </c>
+      <c r="C27" s="23" t="s">
+        <v>474</v>
+      </c>
+      <c r="D27" s="23" t="s">
+        <v>475</v>
+      </c>
+      <c r="E27" s="24" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="19">
+        <v>26</v>
+      </c>
+      <c r="B28" s="20" t="s">
+        <v>476</v>
+      </c>
+      <c r="C28" s="20" t="s">
+        <v>477</v>
+      </c>
+      <c r="D28" s="20" t="s">
+        <v>478</v>
+      </c>
+      <c r="E28" s="21" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="22">
+        <v>28</v>
+      </c>
+      <c r="B29" s="23" t="s">
+        <v>479</v>
+      </c>
+      <c r="C29" s="23" t="s">
+        <v>480</v>
+      </c>
+      <c r="D29" s="23" t="s">
+        <v>452</v>
+      </c>
+      <c r="E29" s="24" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="19">
+        <v>29</v>
+      </c>
+      <c r="B30" s="20" t="s">
+        <v>481</v>
+      </c>
+      <c r="C30" s="20" t="s">
+        <v>482</v>
+      </c>
+      <c r="D30" s="20" t="s">
+        <v>413</v>
+      </c>
+      <c r="E30" s="21" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="22">
+        <v>30</v>
+      </c>
+      <c r="B31" s="23" t="s">
+        <v>483</v>
+      </c>
+      <c r="C31" s="23" t="s">
+        <v>484</v>
+      </c>
+      <c r="D31" s="23" t="s">
+        <v>413</v>
+      </c>
+      <c r="E31" s="24" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="19">
+        <v>31</v>
+      </c>
+      <c r="B32" s="20" t="s">
+        <v>485</v>
+      </c>
+      <c r="C32" s="20" t="s">
+        <v>486</v>
+      </c>
+      <c r="D32" s="20" t="s">
+        <v>462</v>
+      </c>
+      <c r="E32" s="21" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="22">
+        <v>32</v>
+      </c>
+      <c r="B33" s="23" t="s">
+        <v>487</v>
+      </c>
+      <c r="C33" s="23" t="s">
+        <v>488</v>
+      </c>
+      <c r="D33" s="23" t="s">
+        <v>489</v>
+      </c>
+      <c r="E33" s="24" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="19">
+        <v>33</v>
+      </c>
+      <c r="B34" s="20" t="s">
+        <v>491</v>
+      </c>
+      <c r="C34" s="20" t="s">
+        <v>492</v>
+      </c>
+      <c r="D34" s="20" t="s">
+        <v>478</v>
+      </c>
+      <c r="E34" s="21" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="22">
+        <v>34</v>
+      </c>
+      <c r="B35" s="23" t="s">
+        <v>494</v>
+      </c>
+      <c r="C35" s="23" t="s">
+        <v>495</v>
+      </c>
+      <c r="D35" s="23" t="s">
+        <v>478</v>
+      </c>
+      <c r="E35" s="24" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="19">
+        <v>35</v>
+      </c>
+      <c r="B36" s="20" t="s">
+        <v>496</v>
+      </c>
+      <c r="C36" s="20" t="s">
+        <v>497</v>
+      </c>
+      <c r="D36" s="20" t="s">
+        <v>462</v>
+      </c>
+      <c r="E36" s="21" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="22">
+        <v>36</v>
+      </c>
+      <c r="B37" s="23" t="s">
+        <v>498</v>
+      </c>
+      <c r="C37" s="23" t="s">
+        <v>499</v>
+      </c>
+      <c r="D37" s="23" t="s">
+        <v>459</v>
+      </c>
+      <c r="E37" s="24" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="19">
+        <v>37</v>
+      </c>
+      <c r="B38" s="20" t="s">
+        <v>500</v>
+      </c>
+      <c r="C38" s="20" t="s">
+        <v>501</v>
+      </c>
+      <c r="D38" s="20" t="s">
+        <v>413</v>
+      </c>
+      <c r="E38" s="21" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="22">
+        <v>38</v>
+      </c>
+      <c r="B39" s="23" t="s">
+        <v>502</v>
+      </c>
+      <c r="C39" s="23" t="s">
+        <v>503</v>
+      </c>
+      <c r="D39" s="23" t="s">
+        <v>504</v>
+      </c>
+      <c r="E39" s="24" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="19">
+        <v>38</v>
+      </c>
+      <c r="B40" s="20" t="s">
+        <v>505</v>
+      </c>
+      <c r="C40" s="20" t="s">
+        <v>506</v>
+      </c>
+      <c r="D40" s="20" t="s">
+        <v>452</v>
+      </c>
+      <c r="E40" s="21" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="28">
+        <v>38</v>
+      </c>
+      <c r="B41" s="29" t="s">
+        <v>507</v>
+      </c>
+      <c r="C41" s="29" t="s">
+        <v>508</v>
+      </c>
+      <c r="D41" s="29" t="s">
+        <v>478</v>
+      </c>
+      <c r="E41" s="30" t="s">
+        <v>374</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>410</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="31">
+        <v>1</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>509</v>
+      </c>
+      <c r="C2" s="31" t="s">
+        <v>510</v>
+      </c>
+      <c r="D2" s="31">
+        <v>48430</v>
+      </c>
+      <c r="E2" s="31" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="31">
+        <v>2</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>512</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>513</v>
+      </c>
+      <c r="D3" s="31">
+        <v>51164</v>
+      </c>
+      <c r="E3" s="31" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="31">
+        <v>3</v>
+      </c>
+      <c r="B4" s="31" t="s">
+        <v>515</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>516</v>
+      </c>
+      <c r="D4" s="31">
+        <v>97336</v>
+      </c>
+      <c r="E4" s="31" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="31">
+        <v>3</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>518</v>
+      </c>
+      <c r="C5" s="31" t="s">
+        <v>519</v>
+      </c>
+      <c r="D5" s="31">
+        <v>44176</v>
+      </c>
+      <c r="E5" s="31" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="31">
+        <v>5</v>
+      </c>
+      <c r="B6" s="31" t="s">
+        <v>521</v>
+      </c>
+      <c r="C6" s="31" t="s">
+        <v>522</v>
+      </c>
+      <c r="D6" s="31">
+        <v>56691</v>
+      </c>
+      <c r="E6" s="31" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="31">
+        <v>6</v>
+      </c>
+      <c r="B7" s="31" t="s">
+        <v>523</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>524</v>
+      </c>
+      <c r="D7" s="31">
+        <v>120750</v>
+      </c>
+      <c r="E7" s="31" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="31">
+        <v>7</v>
+      </c>
+      <c r="B8" s="31" t="s">
+        <v>526</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>527</v>
+      </c>
+      <c r="D8" s="31">
+        <v>105571</v>
+      </c>
+      <c r="E8" s="31" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="31">
+        <v>8</v>
+      </c>
+      <c r="B9" s="31" t="s">
+        <v>529</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>530</v>
+      </c>
+      <c r="D9" s="31">
+        <v>115001</v>
+      </c>
+      <c r="E9" s="31" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="31">
+        <v>9</v>
+      </c>
+      <c r="B10" s="31" t="s">
+        <v>531</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>532</v>
+      </c>
+      <c r="D10" s="31">
+        <v>108063</v>
+      </c>
+      <c r="E10" s="31" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="31">
+        <v>10</v>
+      </c>
+      <c r="B11" s="31" t="s">
+        <v>534</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>535</v>
+      </c>
+      <c r="D11" s="31">
+        <v>53920</v>
+      </c>
+      <c r="E11" s="31" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="31">
+        <v>11</v>
+      </c>
+      <c r="B12" s="31" t="s">
+        <v>537</v>
+      </c>
+      <c r="C12" s="31" t="s">
+        <v>538</v>
+      </c>
+      <c r="D12" s="31">
+        <v>54485</v>
+      </c>
+      <c r="E12" s="31" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="31">
+        <v>12</v>
+      </c>
+      <c r="B13" s="31" t="s">
+        <v>539</v>
+      </c>
+      <c r="C13" s="31" t="s">
+        <v>540</v>
+      </c>
+      <c r="D13" s="31">
+        <v>137072</v>
+      </c>
+      <c r="E13" s="31" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="31">
+        <v>13</v>
+      </c>
+      <c r="B14" s="31" t="s">
+        <v>541</v>
+      </c>
+      <c r="C14" s="31" t="s">
+        <v>542</v>
+      </c>
+      <c r="D14" s="31">
+        <v>105465</v>
+      </c>
+      <c r="E14" s="31" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="31">
+        <v>14</v>
+      </c>
+      <c r="B15" s="31" t="s">
+        <v>543</v>
+      </c>
+      <c r="C15" s="31" t="s">
+        <v>544</v>
+      </c>
+      <c r="D15" s="31">
+        <v>137148</v>
+      </c>
+      <c r="E15" s="31" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="31">
+        <v>15</v>
+      </c>
+      <c r="B16" s="31" t="s">
+        <v>546</v>
+      </c>
+      <c r="C16" s="31" t="s">
+        <v>547</v>
+      </c>
+      <c r="D16" s="31">
+        <v>111655</v>
+      </c>
+      <c r="E16" s="31" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="31">
+        <v>16</v>
+      </c>
+      <c r="B17" s="31" t="s">
+        <v>549</v>
+      </c>
+      <c r="C17" s="31" t="s">
+        <v>530</v>
+      </c>
+      <c r="D17" s="31">
+        <v>102598</v>
+      </c>
+      <c r="E17" s="31" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="31">
+        <v>17</v>
+      </c>
+      <c r="B18" s="31" t="s">
+        <v>550</v>
+      </c>
+      <c r="C18" s="31" t="s">
+        <v>551</v>
+      </c>
+      <c r="D18" s="31">
+        <v>111664</v>
+      </c>
+      <c r="E18" s="31" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="31">
+        <v>18</v>
+      </c>
+      <c r="B19" s="31" t="s">
+        <v>553</v>
+      </c>
+      <c r="C19" s="31" t="s">
+        <v>554</v>
+      </c>
+      <c r="D19" s="31">
+        <v>49260</v>
+      </c>
+      <c r="E19" s="31" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="31">
+        <v>19</v>
+      </c>
+      <c r="B20" s="31" t="s">
+        <v>555</v>
+      </c>
+      <c r="C20" s="31" t="s">
+        <v>556</v>
+      </c>
+      <c r="D20" s="31">
+        <v>99978</v>
+      </c>
+      <c r="E20" s="31" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="31">
+        <v>20</v>
+      </c>
+      <c r="B21" s="31" t="s">
+        <v>557</v>
+      </c>
+      <c r="C21" s="31" t="s">
+        <v>558</v>
+      </c>
+      <c r="D21" s="31">
+        <v>94439</v>
+      </c>
+      <c r="E21" s="31" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="31">
+        <v>21</v>
+      </c>
+      <c r="B22" s="31" t="s">
+        <v>559</v>
+      </c>
+      <c r="C22" s="31" t="s">
+        <v>560</v>
+      </c>
+      <c r="D22" s="31">
+        <v>31265</v>
+      </c>
+      <c r="E22" s="31" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="31">
+        <v>22</v>
+      </c>
+      <c r="B23" s="31" t="s">
+        <v>561</v>
+      </c>
+      <c r="C23" s="31" t="s">
+        <v>562</v>
+      </c>
+      <c r="D23" s="31">
+        <v>120166</v>
+      </c>
+      <c r="E23" s="31" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="31">
+        <v>23</v>
+      </c>
+      <c r="B24" s="31" t="s">
+        <v>564</v>
+      </c>
+      <c r="C24" s="31" t="s">
+        <v>565</v>
+      </c>
+      <c r="D24" s="31">
+        <v>117173</v>
+      </c>
+      <c r="E24" s="31" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="31">
+        <v>24</v>
+      </c>
+      <c r="B25" s="31" t="s">
+        <v>567</v>
+      </c>
+      <c r="C25" s="31" t="s">
+        <v>568</v>
+      </c>
+      <c r="D25" s="31">
+        <v>113352</v>
+      </c>
+      <c r="E25" s="31" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="31">
+        <v>25</v>
+      </c>
+      <c r="B26" s="31" t="s">
+        <v>570</v>
+      </c>
+      <c r="C26" s="31" t="s">
+        <v>571</v>
+      </c>
+      <c r="D26" s="31">
+        <v>102584</v>
+      </c>
+      <c r="E26" s="31" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="31">
+        <v>26</v>
+      </c>
+      <c r="B27" s="31" t="s">
+        <v>572</v>
+      </c>
+      <c r="C27" s="31" t="s">
+        <v>573</v>
+      </c>
+      <c r="D27" s="31">
+        <v>46629</v>
+      </c>
+      <c r="E27" s="31" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="31">
+        <v>27</v>
+      </c>
+      <c r="B28" s="31" t="s">
+        <v>574</v>
+      </c>
+      <c r="C28" s="31" t="s">
+        <v>575</v>
+      </c>
+      <c r="D28" s="31">
+        <v>112812</v>
+      </c>
+      <c r="E28" s="31" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="31">
+        <v>28</v>
+      </c>
+      <c r="B29" s="31" t="s">
+        <v>576</v>
+      </c>
+      <c r="C29" s="31" t="s">
+        <v>527</v>
+      </c>
+      <c r="D29" s="31">
+        <v>116053</v>
+      </c>
+      <c r="E29" s="31" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="31">
+        <v>29</v>
+      </c>
+      <c r="B30" s="31" t="s">
+        <v>577</v>
+      </c>
+      <c r="C30" s="31" t="s">
+        <v>578</v>
+      </c>
+      <c r="D30" s="31">
+        <v>115411</v>
+      </c>
+      <c r="E30" s="31" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="31">
+        <v>29</v>
+      </c>
+      <c r="B31" s="31" t="s">
+        <v>580</v>
+      </c>
+      <c r="C31" s="31" t="s">
+        <v>581</v>
+      </c>
+      <c r="D31" s="31">
+        <v>112733</v>
+      </c>
+      <c r="E31" s="31" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="31">
+        <v>31</v>
+      </c>
+      <c r="B32" s="31" t="s">
+        <v>582</v>
+      </c>
+      <c r="C32" s="31" t="s">
+        <v>583</v>
+      </c>
+      <c r="D32" s="31">
+        <v>137130</v>
+      </c>
+      <c r="E32" s="31" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="31">
+        <v>32</v>
+      </c>
+      <c r="B33" s="31" t="s">
+        <v>585</v>
+      </c>
+      <c r="C33" s="31" t="s">
+        <v>586</v>
+      </c>
+      <c r="D33" s="31">
+        <v>115213</v>
+      </c>
+      <c r="E33" s="31" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="31">
+        <v>33</v>
+      </c>
+      <c r="B34" s="31" t="s">
+        <v>587</v>
+      </c>
+      <c r="C34" s="31" t="s">
+        <v>588</v>
+      </c>
+      <c r="D34" s="31">
+        <v>113278</v>
+      </c>
+      <c r="E34" s="31" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="31">
+        <v>34</v>
+      </c>
+      <c r="B35" s="31" t="s">
+        <v>589</v>
+      </c>
+      <c r="C35" s="31" t="s">
+        <v>590</v>
+      </c>
+      <c r="D35" s="31">
+        <v>92271</v>
+      </c>
+      <c r="E35" s="31" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="31">
+        <v>35</v>
+      </c>
+      <c r="B36" s="31" t="s">
+        <v>592</v>
+      </c>
+      <c r="C36" s="31" t="s">
+        <v>593</v>
+      </c>
+      <c r="D36" s="31">
+        <v>132481</v>
+      </c>
+      <c r="E36" s="31" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="31">
+        <v>36</v>
+      </c>
+      <c r="B37" s="31" t="s">
+        <v>595</v>
+      </c>
+      <c r="C37" s="31" t="s">
+        <v>596</v>
+      </c>
+      <c r="D37" s="31">
+        <v>101930</v>
+      </c>
+      <c r="E37" s="31" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="31">
+        <v>37</v>
+      </c>
+      <c r="B38" s="31" t="s">
+        <v>597</v>
+      </c>
+      <c r="C38" s="31" t="s">
+        <v>598</v>
+      </c>
+      <c r="D38" s="31">
+        <v>122300</v>
+      </c>
+      <c r="E38" s="31" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="31">
+        <v>38</v>
+      </c>
+      <c r="B39" s="31" t="s">
+        <v>599</v>
+      </c>
+      <c r="C39" s="31" t="s">
+        <v>600</v>
+      </c>
+      <c r="D39" s="31">
+        <v>94905</v>
+      </c>
+      <c r="E39" s="31" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="31">
+        <v>39</v>
+      </c>
+      <c r="B40" s="31" t="s">
+        <v>601</v>
+      </c>
+      <c r="C40" s="31" t="s">
+        <v>602</v>
+      </c>
+      <c r="D40" s="31">
+        <v>135525</v>
+      </c>
+      <c r="E40" s="31" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="31">
+        <v>40</v>
+      </c>
+      <c r="B41" s="31" t="s">
+        <v>603</v>
+      </c>
+      <c r="C41" s="31" t="s">
+        <v>604</v>
+      </c>
+      <c r="D41" s="31">
+        <v>104321</v>
+      </c>
+      <c r="E41" s="31" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="31">
+        <v>41</v>
+      </c>
+      <c r="B42" s="31" t="s">
+        <v>605</v>
+      </c>
+      <c r="C42" s="31" t="s">
+        <v>606</v>
+      </c>
+      <c r="D42" s="31">
+        <v>124092</v>
+      </c>
+      <c r="E42" s="31" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="31">
+        <v>41</v>
+      </c>
+      <c r="B43" s="31" t="s">
+        <v>607</v>
+      </c>
+      <c r="C43" s="31" t="s">
+        <v>608</v>
+      </c>
+      <c r="D43" s="31">
+        <v>122619</v>
+      </c>
+      <c r="E43" s="31" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="31">
+        <v>43</v>
+      </c>
+      <c r="B44" s="31" t="s">
+        <v>609</v>
+      </c>
+      <c r="C44" s="31" t="s">
+        <v>610</v>
+      </c>
+      <c r="D44" s="31">
+        <v>115340</v>
+      </c>
+      <c r="E44" s="31" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="31">
+        <v>44</v>
+      </c>
+      <c r="B45" s="31" t="s">
+        <v>611</v>
+      </c>
+      <c r="C45" s="31" t="s">
+        <v>513</v>
+      </c>
+      <c r="D45" s="31">
+        <v>104743</v>
+      </c>
+      <c r="E45" s="31" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="31">
+        <v>45</v>
+      </c>
+      <c r="B46" s="31" t="s">
+        <v>612</v>
+      </c>
+      <c r="C46" s="31" t="s">
+        <v>538</v>
+      </c>
+      <c r="D46" s="31">
+        <v>105113</v>
+      </c>
+      <c r="E46" s="31" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="31">
+        <v>46</v>
+      </c>
+      <c r="B47" s="31" t="s">
+        <v>614</v>
+      </c>
+      <c r="C47" s="31" t="s">
+        <v>615</v>
+      </c>
+      <c r="D47" s="31">
+        <v>127703</v>
+      </c>
+      <c r="E47" s="31" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="31">
+        <v>47</v>
+      </c>
+      <c r="B48" s="31" t="s">
+        <v>617</v>
+      </c>
+      <c r="C48" s="31" t="s">
+        <v>586</v>
+      </c>
+      <c r="D48" s="31">
+        <v>130361</v>
+      </c>
+      <c r="E48" s="31" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="31">
+        <v>47</v>
+      </c>
+      <c r="B49" s="31" t="s">
+        <v>618</v>
+      </c>
+      <c r="C49" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="D49" s="31">
+        <v>122846</v>
+      </c>
+      <c r="E49" s="31" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="31">
+        <v>49</v>
+      </c>
+      <c r="B50" s="31" t="s">
+        <v>620</v>
+      </c>
+      <c r="C50" s="31" t="s">
+        <v>621</v>
+      </c>
+      <c r="D50" s="31">
+        <v>118970</v>
+      </c>
+      <c r="E50" s="31" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="31">
+        <v>50</v>
+      </c>
+      <c r="B51" s="31" t="s">
+        <v>623</v>
+      </c>
+      <c r="C51" s="31" t="s">
+        <v>530</v>
+      </c>
+      <c r="D51" s="31">
+        <v>120441</v>
+      </c>
+      <c r="E51" s="31" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="31">
+        <v>51</v>
+      </c>
+      <c r="B52" s="31" t="s">
+        <v>624</v>
+      </c>
+      <c r="C52" s="31" t="s">
+        <v>575</v>
+      </c>
+      <c r="D52" s="31">
+        <v>56232</v>
+      </c>
+      <c r="E52" s="31" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="31">
+        <v>51</v>
+      </c>
+      <c r="B53" s="31" t="s">
+        <v>625</v>
+      </c>
+      <c r="C53" s="31" t="s">
+        <v>626</v>
+      </c>
+      <c r="D53" s="31">
+        <v>133196</v>
+      </c>
+      <c r="E53" s="31" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="31">
+        <v>53</v>
+      </c>
+      <c r="B54" s="31" t="s">
+        <v>627</v>
+      </c>
+      <c r="C54" s="31" t="s">
+        <v>600</v>
+      </c>
+      <c r="D54" s="31">
+        <v>110468</v>
+      </c>
+      <c r="E54" s="31" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="31">
+        <v>54</v>
+      </c>
+      <c r="B55" s="31" t="s">
+        <v>628</v>
+      </c>
+      <c r="C55" s="31" t="s">
+        <v>629</v>
+      </c>
+      <c r="D55" s="31">
+        <v>105233</v>
+      </c>
+      <c r="E55" s="31" t="s">
+        <v>630</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>